<commit_message>
moving formula list needed for ulam out of script and into a function
</commit_message>
<xml_diff>
--- a/example model control.xlsx
+++ b/example model control.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\R\tidymmm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3490E25-5180-41A5-96AA-D051FA1DC5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56705BC3-DD10-4796-A794-97565AF0EAC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{E15138B5-0913-440B-A52B-3172F9D245BA}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{E15138B5-0913-440B-A52B-3172F9D245BA}"/>
   </bookViews>
   <sheets>
     <sheet name="workflow" sheetId="3" r:id="rId1"/>
@@ -529,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D79CA1B-8D6F-4588-9F7B-E9E2FAF0425E}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -600,7 +600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F036211F-86F5-4F9C-85F9-C4D9573482AB}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed ulam formula error by movign the parse(text=) out into an sapply in the mmm functions.R file
</commit_message>
<xml_diff>
--- a/example model control.xlsx
+++ b/example model control.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\R\tidymmm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56705BC3-DD10-4796-A794-97565AF0EAC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1408DC34-385B-4238-9BE5-58E453192707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{E15138B5-0913-440B-A52B-3172F9D245BA}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{E15138B5-0913-440B-A52B-3172F9D245BA}"/>
   </bookViews>
   <sheets>
     <sheet name="workflow" sheetId="3" r:id="rId1"/>
@@ -529,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D79CA1B-8D6F-4588-9F7B-E9E2FAF0425E}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -558,7 +558,7 @@
         <v>27</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.75">
@@ -600,7 +600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F036211F-86F5-4F9C-85F9-C4D9573482AB}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
continuing to move steps out of a script and into functions
</commit_message>
<xml_diff>
--- a/example model control.xlsx
+++ b/example model control.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\R\tidymmm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1408DC34-385B-4238-9BE5-58E453192707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7397982E-1114-4E17-B6A4-A7EFBBAD29CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{E15138B5-0913-440B-A52B-3172F9D245BA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
   <si>
     <t>start_name</t>
   </si>
@@ -66,9 +66,6 @@
     <t>tv</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>prior</t>
   </si>
   <si>
@@ -175,6 +172,18 @@
   </si>
   <si>
     <t>fft_terms</t>
+  </si>
+  <si>
+    <t>Which variable are we modeling?</t>
+  </si>
+  <si>
+    <t>add_trend</t>
+  </si>
+  <si>
+    <t>Estimate a trend effect using the trend (role 2 = 'trend) variable?</t>
+  </si>
+  <si>
+    <t>trend</t>
   </si>
 </sst>
 </file>
@@ -527,68 +536,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D79CA1B-8D6F-4588-9F7B-E9E2FAF0425E}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="108.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.31640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.31640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>29</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="b">
+        <v>30</v>
+      </c>
+      <c r="B2" t="b">
         <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3">
+        <v>33</v>
+      </c>
+      <c r="B3">
         <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -601,7 +624,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -625,22 +648,22 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.75">
@@ -659,10 +682,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -682,12 +705,12 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -698,22 +721,22 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6">
         <v>-1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J6">
         <v>10</v>
@@ -721,10 +744,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -736,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J7">
         <v>10</v>
@@ -744,10 +767,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -759,7 +782,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J8">
         <v>10</v>
@@ -767,22 +790,22 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J9">
         <v>10</v>
@@ -790,13 +813,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -804,13 +827,13 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -818,16 +841,16 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -859,27 +882,27 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
       <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
       <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>100</v>

</xml_diff>

<commit_message>
minor edits to prove out a run through with tuning and without.
</commit_message>
<xml_diff>
--- a/example model control.xlsx
+++ b/example model control.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\R\tidymmm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7397982E-1114-4E17-B6A4-A7EFBBAD29CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBF959A-C16F-45D3-A14C-5384E6017F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{E15138B5-0913-440B-A52B-3172F9D245BA}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{E15138B5-0913-440B-A52B-3172F9D245BA}"/>
   </bookViews>
   <sheets>
     <sheet name="workflow" sheetId="3" r:id="rId1"/>
     <sheet name="variables" sheetId="1" r:id="rId2"/>
     <sheet name="role controls" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'role controls'!$A$1:$A$42</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
   <si>
     <t>start_name</t>
   </si>
@@ -184,13 +185,19 @@
   </si>
   <si>
     <t>trend</t>
+  </si>
+  <si>
+    <t>time_id</t>
+  </si>
+  <si>
+    <t>time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,13 +205,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -219,9 +240,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D79CA1B-8D6F-4588-9F7B-E9E2FAF0425E}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -564,7 +587,7 @@
         <v>30</v>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
@@ -603,14 +626,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B6" t="b">
+      <c r="B6" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -621,10 +644,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F036211F-86F5-4F9C-85F9-C4D9573482AB}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -701,11 +724,11 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>50</v>
+      <c r="C4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.75">
@@ -851,6 +874,20 @@
       </c>
       <c r="D12" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -864,7 +901,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -949,4 +986,33 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6E1195-CEC0-4F9F-A993-5D4EE2DE15A6}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding in random slopes as an option
</commit_message>
<xml_diff>
--- a/example model control.xlsx
+++ b/example model control.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\R\tidymmm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBF959A-C16F-45D3-A14C-5384E6017F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C3D159-D310-4A0F-B120-F58325A2050F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{E15138B5-0913-440B-A52B-3172F9D245BA}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{E15138B5-0913-440B-A52B-3172F9D245BA}"/>
   </bookViews>
   <sheets>
     <sheet name="workflow" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
   <si>
     <t>start_name</t>
   </si>
@@ -191,6 +191,18 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>random slopes</t>
+  </si>
+  <si>
+    <t>list_rand_slopes</t>
+  </si>
+  <si>
+    <t>(1|store)</t>
+  </si>
+  <si>
+    <t>(TV1|store), (TV2|store)</t>
   </si>
 </sst>
 </file>
@@ -559,19 +571,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D79CA1B-8D6F-4588-9F7B-E9E2FAF0425E}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="108.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.31640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="108.3515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.64453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.29296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -582,7 +595,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -593,29 +606,29 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>33</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -626,7 +639,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="s">
         <v>49</v>
       </c>
@@ -635,6 +648,17 @@
       </c>
       <c r="C6" s="3" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -646,18 +670,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F036211F-86F5-4F9C-85F9-C4D9573482AB}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="35.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.54296875" customWidth="1"/>
-    <col min="4" max="4" width="10.76953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.87890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.52734375" customWidth="1"/>
+    <col min="4" max="4" width="10.76171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -689,7 +713,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -703,7 +727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -717,7 +741,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -731,7 +755,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -742,7 +766,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -765,7 +789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -788,7 +812,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -811,7 +835,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -834,7 +858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -848,7 +872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -862,7 +886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -876,7 +900,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -904,17 +928,17 @@
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.46875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.2265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.52734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.52734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -937,7 +961,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -960,7 +984,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -996,9 +1020,9 @@
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
repairing errors in ulam formula construction with random slopes
</commit_message>
<xml_diff>
--- a/example model control.xlsx
+++ b/example model control.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\R\tidymmm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C3D159-D310-4A0F-B120-F58325A2050F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{873D7FCD-7C51-4973-B36B-A99979E138FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{E15138B5-0913-440B-A52B-3172F9D245BA}"/>
   </bookViews>
@@ -580,7 +580,7 @@
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="108.3515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.64453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1171875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.29296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>